<commit_message>
Configuración de la lógica de Devoluciones
</commit_message>
<xml_diff>
--- a/Documentacion/Product backlog/Product Backlog v1.2/Historias Técnicas versión 1.2.xlsx
+++ b/Documentacion/Product backlog/Product Backlog v1.2/Historias Técnicas versión 1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeteros\Desktop\Proyecto_E-commerce\Documentacion\Product backlog\Product Backlog v1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A273C4-CD4F-45B8-95E4-781E80E94A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06DB1F-E256-4242-A415-128BFCEB13F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1153,22 +1153,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1197,15 +1206,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1DBEB7-C3D2-4473-9B85-4CF26F3AA489}">
   <dimension ref="B1:AJ135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E45"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,16 +1566,16 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1604,14 +1604,14 @@
       <c r="AJ2" s="6"/>
     </row>
     <row r="3" spans="2:36" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -1640,14 +1640,14 @@
       <c r="AJ3" s="6"/>
     </row>
     <row r="4" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -1728,22 +1728,22 @@
       <c r="AJ5" s="6"/>
     </row>
     <row r="6" spans="2:36" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="27" t="s">
         <v>41</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -1783,9 +1783,9 @@
       <c r="B7" s="20"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="15" t="s">
         <v>121</v>
       </c>
@@ -1829,13 +1829,13 @@
       <c r="D8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H8" s="15" t="s">
@@ -1875,9 +1875,9 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="15" t="s">
         <v>123</v>
       </c>
@@ -1921,13 +1921,13 @@
       <c r="D10" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="15" t="s">
@@ -1967,9 +1967,9 @@
       <c r="B11" s="20"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="15" t="s">
         <v>125</v>
       </c>
@@ -2013,13 +2013,13 @@
       <c r="D12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -2059,9 +2059,9 @@
       <c r="B13" s="20"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="15" t="s">
         <v>127</v>
       </c>
@@ -2157,13 +2157,13 @@
       <c r="D15" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="19" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="15" t="s">
@@ -2203,9 +2203,9 @@
       <c r="B16" s="20"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="15" t="s">
         <v>129</v>
       </c>
@@ -2249,13 +2249,13 @@
       <c r="D17" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="15" t="s">
@@ -2295,9 +2295,9 @@
       <c r="B18" s="20"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="15" t="s">
         <v>131</v>
       </c>
@@ -2393,13 +2393,13 @@
       <c r="D20" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="19" t="s">
         <v>28</v>
       </c>
       <c r="H20" s="15" t="s">
@@ -2439,9 +2439,9 @@
       <c r="B21" s="20"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="15" t="s">
         <v>133</v>
       </c>
@@ -2589,13 +2589,13 @@
       <c r="D24" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="19" t="s">
         <v>68</v>
       </c>
       <c r="H24" s="15" t="s">
@@ -2635,9 +2635,9 @@
       <c r="B25" s="20"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
       <c r="H25" s="15" t="s">
         <v>135</v>
       </c>
@@ -2733,13 +2733,13 @@
       <c r="D27" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="24" t="s">
+      <c r="G27" s="19" t="s">
         <v>151</v>
       </c>
       <c r="H27" s="15" t="s">
@@ -2779,9 +2779,9 @@
       <c r="B28" s="20"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
       <c r="H28" s="15" t="s">
         <v>153</v>
       </c>
@@ -2825,13 +2825,13 @@
       <c r="D29" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="19" t="s">
         <v>157</v>
       </c>
       <c r="H29" s="15" t="s">
@@ -2871,9 +2871,9 @@
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
       <c r="H30" s="15" t="s">
         <v>159</v>
       </c>
@@ -2917,13 +2917,13 @@
       <c r="D31" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G31" s="19" t="s">
         <v>163</v>
       </c>
       <c r="H31" s="15" t="s">
@@ -2963,9 +2963,9 @@
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
       <c r="H32" s="15" t="s">
         <v>165</v>
       </c>
@@ -3009,13 +3009,13 @@
       <c r="D33" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="19" t="s">
         <v>169</v>
       </c>
       <c r="H33" s="15" t="s">
@@ -3055,14 +3055,14 @@
       <c r="B34" s="20"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="15" t="s">
         <v>171</v>
       </c>
       <c r="I34" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
@@ -3153,13 +3153,13 @@
       <c r="D36" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="19" t="s">
         <v>180</v>
       </c>
       <c r="H36" s="15" t="s">
@@ -3199,9 +3199,9 @@
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
       <c r="H37" s="15" t="s">
         <v>182</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>83</v>
       </c>
       <c r="I38" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
@@ -3349,13 +3349,13 @@
       <c r="D40" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="24" t="s">
+      <c r="F40" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="24" t="s">
+      <c r="G40" s="19" t="s">
         <v>92</v>
       </c>
       <c r="H40" s="15" t="s">
@@ -3395,9 +3395,9 @@
       <c r="B41" s="20"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
       <c r="H41" s="15" t="s">
         <v>137</v>
       </c>
@@ -3441,13 +3441,13 @@
       <c r="D42" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="24" t="s">
+      <c r="F42" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="19" t="s">
         <v>96</v>
       </c>
       <c r="H42" s="15" t="s">
@@ -3487,9 +3487,9 @@
       <c r="B43" s="20"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
       <c r="H43" s="15" t="s">
         <v>139</v>
       </c>
@@ -3533,13 +3533,13 @@
       <c r="D44" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E44" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G44" s="19" t="s">
         <v>101</v>
       </c>
       <c r="H44" s="15" t="s">
@@ -3579,9 +3579,9 @@
       <c r="B45" s="20"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
       <c r="H45" s="15" t="s">
         <v>141</v>
       </c>
@@ -3625,13 +3625,13 @@
       <c r="D46" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F46" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="24" t="s">
+      <c r="G46" s="19" t="s">
         <v>105</v>
       </c>
       <c r="H46" s="15" t="s">
@@ -3671,9 +3671,9 @@
       <c r="B47" s="20"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
       <c r="H47" s="15" t="s">
         <v>143</v>
       </c>
@@ -3717,13 +3717,13 @@
       <c r="D48" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="24" t="s">
+      <c r="F48" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G48" s="24" t="s">
+      <c r="G48" s="19" t="s">
         <v>108</v>
       </c>
       <c r="H48" s="15" t="s">
@@ -3763,9 +3763,9 @@
       <c r="B49" s="20"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
       <c r="H49" s="15" t="s">
         <v>145</v>
       </c>
@@ -3809,13 +3809,13 @@
       <c r="D50" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F50" s="24" t="s">
+      <c r="F50" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="24" t="s">
+      <c r="G50" s="19" t="s">
         <v>190</v>
       </c>
       <c r="H50" s="18" t="s">
@@ -3855,9 +3855,9 @@
       <c r="B51" s="20"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
       <c r="H51" s="15" t="s">
         <v>192</v>
       </c>
@@ -3901,13 +3901,13 @@
       <c r="D52" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="24" t="s">
+      <c r="E52" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F52" s="24" t="s">
+      <c r="F52" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="24" t="s">
+      <c r="G52" s="19" t="s">
         <v>112</v>
       </c>
       <c r="H52" s="15" t="s">
@@ -3947,9 +3947,9 @@
       <c r="B53" s="20"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
       <c r="H53" s="15" t="s">
         <v>147</v>
       </c>
@@ -3993,13 +3993,13 @@
       <c r="D54" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F54" s="24" t="s">
+      <c r="F54" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="24" t="s">
+      <c r="G54" s="19" t="s">
         <v>112</v>
       </c>
       <c r="H54" s="15" t="s">
@@ -4039,9 +4039,9 @@
       <c r="B55" s="20"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
       <c r="H55" s="15" t="s">
         <v>184</v>
       </c>
@@ -4137,13 +4137,13 @@
       <c r="D57" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="E57" s="24" t="s">
+      <c r="E57" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="24" t="s">
+      <c r="F57" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="24" t="s">
+      <c r="G57" s="19" t="s">
         <v>113</v>
       </c>
       <c r="H57" s="15" t="s">
@@ -4183,9 +4183,9 @@
       <c r="B58" s="20"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
       <c r="H58" s="15" t="s">
         <v>199</v>
       </c>
@@ -4229,13 +4229,13 @@
       <c r="D59" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="E59" s="24" t="s">
+      <c r="E59" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F59" s="24" t="s">
+      <c r="F59" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="24" t="s">
+      <c r="G59" s="19" t="s">
         <v>41</v>
       </c>
       <c r="H59" s="15" t="s">
@@ -4275,9 +4275,9 @@
       <c r="B60" s="20"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
       <c r="H60" s="15" t="s">
         <v>204</v>
       </c>
@@ -4321,13 +4321,13 @@
       <c r="D61" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="E61" s="24" t="s">
+      <c r="E61" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F61" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G61" s="24" t="s">
+      <c r="G61" s="19" t="s">
         <v>180</v>
       </c>
       <c r="H61" s="15" t="s">
@@ -4367,9 +4367,9 @@
       <c r="B62" s="20"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
       <c r="H62" s="15" t="s">
         <v>209</v>
       </c>
@@ -4413,13 +4413,13 @@
       <c r="D63" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E63" s="24" t="s">
+      <c r="E63" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F63" s="24" t="s">
+      <c r="F63" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="24" t="s">
+      <c r="G63" s="19" t="s">
         <v>112</v>
       </c>
       <c r="H63" s="15" t="s">
@@ -4459,9 +4459,9 @@
       <c r="B64" s="20"/>
       <c r="C64" s="22"/>
       <c r="D64" s="22"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="24"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
       <c r="H64" s="15" t="s">
         <v>214</v>
       </c>
@@ -4557,13 +4557,13 @@
       <c r="D66" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E66" s="24" t="s">
+      <c r="E66" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="24" t="s">
+      <c r="F66" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G66" s="24" t="s">
+      <c r="G66" s="19" t="s">
         <v>112</v>
       </c>
       <c r="H66" s="15" t="s">
@@ -4603,9 +4603,9 @@
       <c r="B67" s="20"/>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
       <c r="H67" s="15" t="s">
         <v>223</v>
       </c>
@@ -4649,13 +4649,13 @@
       <c r="D68" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="E68" s="24" t="s">
+      <c r="E68" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="24" t="s">
+      <c r="F68" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G68" s="24" t="s">
+      <c r="G68" s="19" t="s">
         <v>219</v>
       </c>
       <c r="H68" s="18" t="s">
@@ -4695,9 +4695,9 @@
       <c r="B69" s="20"/>
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
       <c r="H69" s="18" t="s">
         <v>228</v>
       </c>
@@ -4741,13 +4741,13 @@
       <c r="D70" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="E70" s="24" t="s">
+      <c r="E70" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F70" s="24" t="s">
+      <c r="F70" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G70" s="24" t="s">
+      <c r="G70" s="19" t="s">
         <v>215</v>
       </c>
       <c r="H70" s="15" t="s">
@@ -4787,9 +4787,9 @@
       <c r="B71" s="20"/>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
       <c r="H71" s="15" t="s">
         <v>233</v>
       </c>
@@ -4833,13 +4833,13 @@
       <c r="D72" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E72" s="24" t="s">
+      <c r="E72" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F72" s="24" t="s">
+      <c r="F72" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G72" s="24" t="s">
+      <c r="G72" s="19" t="s">
         <v>112</v>
       </c>
       <c r="H72" s="15" t="s">
@@ -4879,9 +4879,9 @@
       <c r="B73" s="20"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
       <c r="H73" s="15" t="s">
         <v>238</v>
       </c>
@@ -4925,13 +4925,13 @@
       <c r="D74" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E74" s="24" t="s">
+      <c r="E74" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F74" s="24" t="s">
+      <c r="F74" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G74" s="24" t="s">
+      <c r="G74" s="19" t="s">
         <v>88</v>
       </c>
       <c r="H74" s="15" t="s">
@@ -4968,12 +4968,12 @@
       <c r="AJ74" s="6"/>
     </row>
     <row r="75" spans="2:36" ht="22.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="34"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
       <c r="H75" s="17" t="s">
         <v>241</v>
       </c>
@@ -6689,168 +6689,6 @@
     </row>
   </sheetData>
   <mergeCells count="181">
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -6870,6 +6708,168 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="F72:F73"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I75">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Obtener pedidos, función buscar
</commit_message>
<xml_diff>
--- a/Documentacion/Product backlog/Product Backlog v1.2/Historias Técnicas versión 1.2.xlsx
+++ b/Documentacion/Product backlog/Product Backlog v1.2/Historias Técnicas versión 1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeteros\Desktop\Proyecto_E-commerce\Documentacion\Product backlog\Product Backlog v1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06DB1F-E256-4242-A415-128BFCEB13F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B69CFE-497D-4514-8488-B8322A286CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1153,31 +1153,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1206,6 +1197,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1DBEB7-C3D2-4473-9B85-4CF26F3AA489}">
   <dimension ref="B1:AJ135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:H39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,16 +1566,16 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1604,14 +1604,14 @@
       <c r="AJ2" s="6"/>
     </row>
     <row r="3" spans="2:36" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -1640,14 +1640,14 @@
       <c r="AJ3" s="6"/>
     </row>
     <row r="4" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -1728,22 +1728,22 @@
       <c r="AJ5" s="6"/>
     </row>
     <row r="6" spans="2:36" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="23" t="s">
         <v>41</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -1783,9 +1783,9 @@
       <c r="B7" s="20"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="15" t="s">
         <v>121</v>
       </c>
@@ -1829,13 +1829,13 @@
       <c r="D8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H8" s="15" t="s">
@@ -1875,9 +1875,9 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="15" t="s">
         <v>123</v>
       </c>
@@ -1921,13 +1921,13 @@
       <c r="D10" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="15" t="s">
@@ -1967,9 +1967,9 @@
       <c r="B11" s="20"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="15" t="s">
         <v>125</v>
       </c>
@@ -2013,13 +2013,13 @@
       <c r="D12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -2059,9 +2059,9 @@
       <c r="B13" s="20"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="15" t="s">
         <v>127</v>
       </c>
@@ -2157,13 +2157,13 @@
       <c r="D15" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="24" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="15" t="s">
@@ -2203,9 +2203,9 @@
       <c r="B16" s="20"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="15" t="s">
         <v>129</v>
       </c>
@@ -2249,13 +2249,13 @@
       <c r="D17" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="15" t="s">
@@ -2295,9 +2295,9 @@
       <c r="B18" s="20"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="15" t="s">
         <v>131</v>
       </c>
@@ -2393,13 +2393,13 @@
       <c r="D20" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="24" t="s">
         <v>28</v>
       </c>
       <c r="H20" s="15" t="s">
@@ -2439,9 +2439,9 @@
       <c r="B21" s="20"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="15" t="s">
         <v>133</v>
       </c>
@@ -2589,13 +2589,13 @@
       <c r="D24" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H24" s="15" t="s">
@@ -2635,9 +2635,9 @@
       <c r="B25" s="20"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="15" t="s">
         <v>135</v>
       </c>
@@ -2733,13 +2733,13 @@
       <c r="D27" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="24" t="s">
         <v>151</v>
       </c>
       <c r="H27" s="15" t="s">
@@ -2779,9 +2779,9 @@
       <c r="B28" s="20"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="15" t="s">
         <v>153</v>
       </c>
@@ -2825,13 +2825,13 @@
       <c r="D29" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="24" t="s">
         <v>157</v>
       </c>
       <c r="H29" s="15" t="s">
@@ -2871,9 +2871,9 @@
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="15" t="s">
         <v>159</v>
       </c>
@@ -2917,13 +2917,13 @@
       <c r="D31" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="24" t="s">
         <v>163</v>
       </c>
       <c r="H31" s="15" t="s">
@@ -2963,9 +2963,9 @@
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="15" t="s">
         <v>165</v>
       </c>
@@ -3009,13 +3009,13 @@
       <c r="D33" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="24" t="s">
         <v>169</v>
       </c>
       <c r="H33" s="15" t="s">
@@ -3055,14 +3055,14 @@
       <c r="B34" s="20"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="15" t="s">
         <v>171</v>
       </c>
       <c r="I34" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
@@ -3153,13 +3153,13 @@
       <c r="D36" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="24" t="s">
         <v>180</v>
       </c>
       <c r="H36" s="15" t="s">
@@ -3199,9 +3199,9 @@
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="15" t="s">
         <v>182</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>84</v>
       </c>
       <c r="I39" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
@@ -3349,20 +3349,20 @@
       <c r="D40" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="24" t="s">
         <v>92</v>
       </c>
       <c r="H40" s="15" t="s">
         <v>136</v>
       </c>
       <c r="I40" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
@@ -3395,14 +3395,14 @@
       <c r="B41" s="20"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="15" t="s">
         <v>137</v>
       </c>
       <c r="I41" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
@@ -3441,20 +3441,20 @@
       <c r="D42" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F42" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="24" t="s">
         <v>96</v>
       </c>
       <c r="H42" s="15" t="s">
         <v>138</v>
       </c>
       <c r="I42" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
@@ -3487,14 +3487,14 @@
       <c r="B43" s="20"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
       <c r="H43" s="15" t="s">
         <v>139</v>
       </c>
       <c r="I43" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
@@ -3533,20 +3533,20 @@
       <c r="D44" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="19" t="s">
+      <c r="F44" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="24" t="s">
         <v>101</v>
       </c>
       <c r="H44" s="15" t="s">
         <v>140</v>
       </c>
       <c r="I44" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
@@ -3579,14 +3579,14 @@
       <c r="B45" s="20"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
       <c r="H45" s="15" t="s">
         <v>141</v>
       </c>
       <c r="I45" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
@@ -3625,20 +3625,20 @@
       <c r="D46" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F46" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G46" s="24" t="s">
         <v>105</v>
       </c>
       <c r="H46" s="15" t="s">
         <v>142</v>
       </c>
       <c r="I46" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
@@ -3671,14 +3671,14 @@
       <c r="B47" s="20"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
       <c r="H47" s="15" t="s">
         <v>143</v>
       </c>
       <c r="I47" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -3717,13 +3717,13 @@
       <c r="D48" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G48" s="19" t="s">
+      <c r="G48" s="24" t="s">
         <v>108</v>
       </c>
       <c r="H48" s="15" t="s">
@@ -3763,9 +3763,9 @@
       <c r="B49" s="20"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="15" t="s">
         <v>145</v>
       </c>
@@ -3809,13 +3809,13 @@
       <c r="D50" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F50" s="19" t="s">
+      <c r="F50" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="24" t="s">
         <v>190</v>
       </c>
       <c r="H50" s="18" t="s">
@@ -3855,9 +3855,9 @@
       <c r="B51" s="20"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="15" t="s">
         <v>192</v>
       </c>
@@ -3901,13 +3901,13 @@
       <c r="D52" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F52" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="19" t="s">
+      <c r="G52" s="24" t="s">
         <v>112</v>
       </c>
       <c r="H52" s="15" t="s">
@@ -3947,9 +3947,9 @@
       <c r="B53" s="20"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
       <c r="H53" s="15" t="s">
         <v>147</v>
       </c>
@@ -3993,13 +3993,13 @@
       <c r="D54" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="24" t="s">
         <v>112</v>
       </c>
       <c r="H54" s="15" t="s">
@@ -4039,9 +4039,9 @@
       <c r="B55" s="20"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
       <c r="H55" s="15" t="s">
         <v>184</v>
       </c>
@@ -4137,13 +4137,13 @@
       <c r="D57" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="G57" s="24" t="s">
         <v>113</v>
       </c>
       <c r="H57" s="15" t="s">
@@ -4183,9 +4183,9 @@
       <c r="B58" s="20"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
       <c r="H58" s="15" t="s">
         <v>199</v>
       </c>
@@ -4229,13 +4229,13 @@
       <c r="D59" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F59" s="19" t="s">
+      <c r="F59" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G59" s="24" t="s">
         <v>41</v>
       </c>
       <c r="H59" s="15" t="s">
@@ -4275,9 +4275,9 @@
       <c r="B60" s="20"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
       <c r="H60" s="15" t="s">
         <v>204</v>
       </c>
@@ -4321,13 +4321,13 @@
       <c r="D61" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F61" s="19" t="s">
+      <c r="F61" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="24" t="s">
         <v>180</v>
       </c>
       <c r="H61" s="15" t="s">
@@ -4367,9 +4367,9 @@
       <c r="B62" s="20"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
       <c r="H62" s="15" t="s">
         <v>209</v>
       </c>
@@ -4413,13 +4413,13 @@
       <c r="D63" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F63" s="19" t="s">
+      <c r="F63" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="24" t="s">
         <v>112</v>
       </c>
       <c r="H63" s="15" t="s">
@@ -4459,9 +4459,9 @@
       <c r="B64" s="20"/>
       <c r="C64" s="22"/>
       <c r="D64" s="22"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
       <c r="H64" s="15" t="s">
         <v>214</v>
       </c>
@@ -4557,13 +4557,13 @@
       <c r="D66" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="19" t="s">
+      <c r="F66" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G66" s="19" t="s">
+      <c r="G66" s="24" t="s">
         <v>112</v>
       </c>
       <c r="H66" s="15" t="s">
@@ -4603,9 +4603,9 @@
       <c r="B67" s="20"/>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
       <c r="H67" s="15" t="s">
         <v>223</v>
       </c>
@@ -4649,13 +4649,13 @@
       <c r="D68" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="19" t="s">
+      <c r="F68" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G68" s="19" t="s">
+      <c r="G68" s="24" t="s">
         <v>219</v>
       </c>
       <c r="H68" s="18" t="s">
@@ -4695,9 +4695,9 @@
       <c r="B69" s="20"/>
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
       <c r="H69" s="18" t="s">
         <v>228</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="AI69" s="6"/>
       <c r="AJ69" s="6"/>
     </row>
-    <row r="70" spans="2:36" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:36" ht="22.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="20" t="s">
         <v>229</v>
       </c>
@@ -4741,13 +4741,13 @@
       <c r="D70" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F70" s="19" t="s">
+      <c r="F70" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G70" s="19" t="s">
+      <c r="G70" s="24" t="s">
         <v>215</v>
       </c>
       <c r="H70" s="15" t="s">
@@ -4787,9 +4787,9 @@
       <c r="B71" s="20"/>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="19"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
       <c r="H71" s="15" t="s">
         <v>233</v>
       </c>
@@ -4833,13 +4833,13 @@
       <c r="D72" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E72" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F72" s="19" t="s">
+      <c r="F72" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G72" s="19" t="s">
+      <c r="G72" s="24" t="s">
         <v>112</v>
       </c>
       <c r="H72" s="15" t="s">
@@ -4879,9 +4879,9 @@
       <c r="B73" s="20"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
       <c r="H73" s="15" t="s">
         <v>238</v>
       </c>
@@ -4925,13 +4925,13 @@
       <c r="D74" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F74" s="19" t="s">
+      <c r="F74" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G74" s="19" t="s">
+      <c r="G74" s="24" t="s">
         <v>88</v>
       </c>
       <c r="H74" s="15" t="s">
@@ -4968,12 +4968,12 @@
       <c r="AJ74" s="6"/>
     </row>
     <row r="75" spans="2:36" ht="22.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="21"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
       <c r="H75" s="17" t="s">
         <v>241</v>
       </c>
@@ -6689,6 +6689,168 @@
     </row>
   </sheetData>
   <mergeCells count="181">
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -6708,168 +6870,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="F72:F73"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I75">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>